<commit_message>
Mais uma revisão e adição de arquivos no Scrum GPR
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco (Scrum).xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/Quadro de Gerenciamento de Risco (Scrum).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="123820"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25808"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Dropbox\UFG\GitHubProjects\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Genérico\2-Gerencia de Projeto\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viniciuscmac/Desktop/GitHub/P.I.-ES-UFG-2015-BIJLMMV/Artefatos de Documentação/Processo Aplicado/EveRemind/2-Gerencia de Projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29260" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="4" r:id="rId1"/>
@@ -31,13 +31,18 @@
     <definedName name="Status">Valores!#REF!</definedName>
     <definedName name="Urgencia">Valores!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <webPublishing codePage="1252"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Severidade</t>
   </si>
@@ -85,6 +90,66 @@
   </si>
   <si>
     <t>2  -Média</t>
+  </si>
+  <si>
+    <t>Atraso da Entrega da Sprint</t>
+  </si>
+  <si>
+    <t>Estouro do Orçamento</t>
+  </si>
+  <si>
+    <t>O estouro no orçamento acaba culminando em um replanejamento do projeto e das tarefas seguintes.</t>
+  </si>
+  <si>
+    <t>O atraso da entrega pode comprometer todo o cronograma previamente estipulado.</t>
+  </si>
+  <si>
+    <t>Desistência de Algum Membro do Projeto</t>
+  </si>
+  <si>
+    <t>Caso algum membro desista os outros devem dividir o que o desistente iria fazer, e replanejar as horas dedicada.</t>
+  </si>
+  <si>
+    <t>Resultado Desaprovado pelo PO</t>
+  </si>
+  <si>
+    <t>Caso o PO desaprove o resultado da sprint, todo o projeto deve ser replanejado, incluindo datas.</t>
+  </si>
+  <si>
+    <t>Equipe Inexperiente</t>
+  </si>
+  <si>
+    <t>Falta de treinamento com Ferramentas</t>
+  </si>
+  <si>
+    <t>Por ser uma equipe nova, a inexperiência irá alocar mais tempo para aprendizado.</t>
+  </si>
+  <si>
+    <t>Algumas ferramentas utilizadas necessitam de aprendizado pela equipe.</t>
+  </si>
+  <si>
+    <t>Documentação Atrasada</t>
+  </si>
+  <si>
+    <t>Se a documentação do projeto atrasar, não será possível prosseguir com outras áreas.</t>
+  </si>
+  <si>
+    <t>Impossibilidade de Reunião</t>
+  </si>
+  <si>
+    <t>Algum membro pode não estar disponível para qualquer das reuniões</t>
+  </si>
+  <si>
+    <t>Quantidade Alta de Defeitos</t>
+  </si>
+  <si>
+    <t>Os defeitos no software a ser entregue pode ser grande, comprometendo a entrega.</t>
+  </si>
+  <si>
+    <t>Não Cumprimento de Tarefas</t>
+  </si>
+  <si>
+    <t>Algum membro pode não cumprir o que for alocado para o mesmo realizar.</t>
   </si>
 </sst>
 </file>
@@ -484,16 +549,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,20 +671,20 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -628,21 +693,21 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -650,14 +715,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -782,64 +847,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
+    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
+    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
+    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
+    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
+    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Nota" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
-    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
-    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="80">
     <dxf>
@@ -1567,9 +1632,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1607,7 +1672,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1679,7 +1744,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1853,28 +1918,28 @@
   <dimension ref="B1:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="29.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="4"/>
       <c r="D1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="18" t="s">
         <v>6</v>
       </c>
@@ -1894,150 +1959,226 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="60" x14ac:dyDescent="0.2">
       <c r="B3" s="20">
         <v>1</v>
       </c>
       <c r="C3" s="19">
         <f t="shared" ref="C3:C17" si="0">$E3+$F3</f>
+        <v>5</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="21">
+        <v>3</v>
+      </c>
+      <c r="F3" s="21">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21">
-        <v>1</v>
-      </c>
-      <c r="F3" s="21">
-        <v>1</v>
-      </c>
-      <c r="G3" s="20"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.2">
       <c r="B4" s="21">
         <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21">
+        <v>2</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="B5" s="21">
         <f t="shared" ref="B5:B17" si="1">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21">
+        <v>2</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="B6" s="21">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C6" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <v>3</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B7" s="21">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C7" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="21">
+        <v>3</v>
+      </c>
+      <c r="F7" s="21">
+        <v>3</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B8" s="21">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="21">
+        <v>1</v>
+      </c>
+      <c r="F8" s="21">
+        <v>1</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B9" s="21">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C9" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="21">
+        <v>2</v>
+      </c>
+      <c r="F9" s="21">
+        <v>3</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B10" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C10" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="21">
+        <v>3</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B11" s="21">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C11" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="21">
+        <v>2</v>
+      </c>
+      <c r="F11" s="21">
+        <v>3</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="B12" s="21">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="21">
+        <v>3</v>
+      </c>
+      <c r="F12" s="21">
+        <v>3</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="21">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2051,7 +2192,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B14" s="21">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2065,7 +2206,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2079,7 +2220,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="21">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2093,7 +2234,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="21">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2107,17 +2248,17 @@
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="10"/>
     </row>
   </sheetData>
@@ -2394,14 +2535,14 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2411,7 +2552,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3">
         <f>B4+1</f>
         <v>3</v>
@@ -2429,7 +2570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <f>B5+1</f>
         <v>2</v>
@@ -2447,7 +2588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2464,7 +2605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2518,16 +2659,16 @@
       <selection activeCell="AQ33" sqref="AQ33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -2538,14 +2679,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
@@ -2556,7 +2697,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
@@ -2567,7 +2708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
@@ -2578,14 +2719,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>

</xml_diff>